<commit_message>
Restore original simultaneous logic with 16:00 exit window
</commit_message>
<xml_diff>
--- a/trade_log.xlsx
+++ b/trade_log.xlsx
@@ -460,17 +460,17 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>PnL</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Result</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Close</t>
         </is>
       </c>
     </row>
@@ -490,15 +490,15 @@
         <v>6699.77978515625</v>
       </c>
       <c r="E2" t="n">
+        <v>6699.77978515625</v>
+      </c>
+      <c r="F2" t="n">
         <v>21.3896484375</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>6699.77978515625</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -517,15 +517,15 @@
         <v>6738.169921875</v>
       </c>
       <c r="E3" t="n">
+        <v>6738.169921875</v>
+      </c>
+      <c r="F3" t="n">
         <v>9.06005859375</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>6738.169921875</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -544,15 +544,15 @@
         <v>6791.14013671875</v>
       </c>
       <c r="E4" t="n">
+        <v>6791.14013671875</v>
+      </c>
+      <c r="F4" t="n">
         <v>8.6396484375</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>6791.14013671875</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -571,15 +571,15 @@
         <v>6890.89013671875</v>
       </c>
       <c r="E5" t="n">
+        <v>6890.89013671875</v>
+      </c>
+      <c r="F5" t="n">
         <v>0</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Flat</t>
         </is>
-      </c>
-      <c r="G5" t="n">
-        <v>6890.89013671875</v>
       </c>
     </row>
     <row r="6">
@@ -598,15 +598,15 @@
         <v>6892.169921875</v>
       </c>
       <c r="E6" t="n">
+        <v>6892.169921875</v>
+      </c>
+      <c r="F6" t="n">
         <v>-7.0400390625</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Loss</t>
         </is>
-      </c>
-      <c r="G6" t="n">
-        <v>6892.169921875</v>
       </c>
     </row>
     <row r="7">
@@ -625,15 +625,15 @@
         <v>6772.39990234375</v>
       </c>
       <c r="E7" t="n">
+        <v>6772.39990234375</v>
+      </c>
+      <c r="F7" t="n">
         <v>-9.06005859375</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Loss</t>
         </is>
-      </c>
-      <c r="G7" t="n">
-        <v>6772.39990234375</v>
       </c>
     </row>
     <row r="8">
@@ -652,15 +652,15 @@
         <v>6831.81982421875</v>
       </c>
       <c r="E8" t="n">
+        <v>6831.81982421875</v>
+      </c>
+      <c r="F8" t="n">
         <v>5.2802734375</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>6831.81982421875</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -679,15 +679,15 @@
         <v>6848.08984375</v>
       </c>
       <c r="E9" t="n">
+        <v>6848.08984375</v>
+      </c>
+      <c r="F9" t="n">
         <v>2.5703125</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>6848.08984375</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -706,15 +706,15 @@
         <v>6738.52001953125</v>
       </c>
       <c r="E10" t="n">
+        <v>6738.52001953125</v>
+      </c>
+      <c r="F10" t="n">
         <v>2.14013671875</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>6738.52001953125</v>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -733,15 +733,15 @@
         <v>6672.91015625</v>
       </c>
       <c r="E11" t="n">
+        <v>6672.91015625</v>
+      </c>
+      <c r="F11" t="n">
         <v>16.3203125</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>6672.91015625</v>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -760,15 +760,15 @@
         <v>6616.93994140625</v>
       </c>
       <c r="E12" t="n">
+        <v>6616.93994140625</v>
+      </c>
+      <c r="F12" t="n">
         <v>38.490234375</v>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>6616.93994140625</v>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -787,15 +787,15 @@
         <v>6603.7998046875</v>
       </c>
       <c r="E13" t="n">
+        <v>6603.7998046875</v>
+      </c>
+      <c r="F13" t="n">
         <v>28.38037109375</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>6603.7998046875</v>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -814,15 +814,15 @@
         <v>6850.509765625</v>
       </c>
       <c r="E14" t="n">
+        <v>6850.509765625</v>
+      </c>
+      <c r="F14" t="n">
         <v>7.73046875</v>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
-        <v>6850.509765625</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -841,15 +841,15 @@
         <v>6847.83984375</v>
       </c>
       <c r="E15" t="n">
+        <v>6847.83984375</v>
+      </c>
+      <c r="F15" t="n">
         <v>10.349609375</v>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>6847.83984375</v>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -868,15 +868,15 @@
         <v>6902.10009765625</v>
       </c>
       <c r="E16" t="n">
+        <v>6902.10009765625</v>
+      </c>
+      <c r="F16" t="n">
         <v>-7.18017578125</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>Loss</t>
         </is>
-      </c>
-      <c r="G16" t="n">
-        <v>6902.10009765625</v>
       </c>
     </row>
     <row r="17">
@@ -895,15 +895,15 @@
         <v>6798.509765625</v>
       </c>
       <c r="E17" t="n">
+        <v>6798.509765625</v>
+      </c>
+      <c r="F17" t="n">
         <v>11.08984375</v>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
-        <v>6798.509765625</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -922,15 +922,15 @@
         <v>6722.22021484375</v>
       </c>
       <c r="E18" t="n">
+        <v>6722.22021484375</v>
+      </c>
+      <c r="F18" t="n">
         <v>-14.44970703125</v>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>Loss</t>
         </is>
-      </c>
-      <c r="G18" t="n">
-        <v>6722.22021484375</v>
       </c>
     </row>
     <row r="19">
@@ -949,15 +949,15 @@
         <v>6774.35009765625</v>
       </c>
       <c r="E19" t="n">
+        <v>6774.35009765625</v>
+      </c>
+      <c r="F19" t="n">
         <v>-8.330078125</v>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>Loss</t>
         </is>
-      </c>
-      <c r="G19" t="n">
-        <v>6774.35009765625</v>
       </c>
     </row>
     <row r="20">
@@ -976,15 +976,15 @@
         <v>6909.02001953125</v>
       </c>
       <c r="E20" t="n">
+        <v>6909.02001953125</v>
+      </c>
+      <c r="F20" t="n">
         <v>-3.18017578125</v>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>Loss</t>
         </is>
-      </c>
-      <c r="G20" t="n">
-        <v>6909.02001953125</v>
       </c>
     </row>
     <row r="21">
@@ -1003,15 +1003,15 @@
         <v>6858.5400390625</v>
       </c>
       <c r="E21" t="n">
+        <v>6858.5400390625</v>
+      </c>
+      <c r="F21" t="n">
         <v>8.419921875</v>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
-        <v>6858.5400390625</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1030,15 +1030,15 @@
         <v>6946.330078125</v>
       </c>
       <c r="E22" t="n">
+        <v>6946.330078125</v>
+      </c>
+      <c r="F22" t="n">
         <v>-1.89013671875</v>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>Loss</t>
         </is>
-      </c>
-      <c r="G22" t="n">
-        <v>6946.330078125</v>
       </c>
     </row>
     <row r="23">
@@ -1057,15 +1057,15 @@
         <v>6965.990234375</v>
       </c>
       <c r="E23" t="n">
+        <v>6965.990234375</v>
+      </c>
+      <c r="F23" t="n">
         <v>7.7197265625</v>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G23" t="n">
-        <v>6965.990234375</v>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1084,15 +1084,15 @@
         <v>6976.72021484375</v>
       </c>
       <c r="E24" t="n">
+        <v>6976.72021484375</v>
+      </c>
+      <c r="F24" t="n">
         <v>2.1796875</v>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G24" t="n">
-        <v>6976.72021484375</v>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1111,15 +1111,15 @@
         <v>6962.97998046875</v>
       </c>
       <c r="E25" t="n">
+        <v>6962.97998046875</v>
+      </c>
+      <c r="F25" t="n">
         <v>9.60986328125</v>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
-        <v>6962.97998046875</v>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1138,15 +1138,15 @@
         <v>6928.41015625</v>
       </c>
       <c r="E26" t="n">
+        <v>6928.41015625</v>
+      </c>
+      <c r="F26" t="n">
         <v>35.3603515625</v>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="G26" t="n">
-        <v>6928.41015625</v>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update entry to 2-bar confirmation and next-bar open
</commit_message>
<xml_diff>
--- a/trade_log.xlsx
+++ b/trade_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6678.39013671875</v>
+        <v>6678.3701171875</v>
       </c>
       <c r="D2" t="n">
         <v>6699.77978515625</v>
@@ -493,7 +493,7 @@
         <v>6699.77978515625</v>
       </c>
       <c r="F2" t="n">
-        <v>21.3896484375</v>
+        <v>21.40966796875</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6747.22998046875</v>
+        <v>6747.14990234375</v>
       </c>
       <c r="D3" t="n">
         <v>6738.169921875</v>
@@ -520,7 +520,7 @@
         <v>6738.169921875</v>
       </c>
       <c r="F3" t="n">
-        <v>9.06005859375</v>
+        <v>8.97998046875</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>6799.77978515625</v>
+        <v>6804.06005859375</v>
       </c>
       <c r="D4" t="n">
         <v>6791.14013671875</v>
@@ -547,7 +547,7 @@
         <v>6791.14013671875</v>
       </c>
       <c r="F4" t="n">
-        <v>8.6396484375</v>
+        <v>12.919921875</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -557,34 +557,34 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SHORT</t>
+          <t>LONG</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6890.89013671875</v>
+        <v>6899.18017578125</v>
       </c>
       <c r="D5" t="n">
-        <v>6890.89013671875</v>
+        <v>6892.169921875</v>
       </c>
       <c r="E5" t="n">
-        <v>6890.89013671875</v>
+        <v>6892.169921875</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>-7.01025390625</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Flat</t>
+          <t>Loss</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45959</v>
+        <v>45961</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -592,20 +592,20 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6899.2099609375</v>
+        <v>6829.7001953125</v>
       </c>
       <c r="D6" t="n">
-        <v>6892.169921875</v>
+        <v>6840.22998046875</v>
       </c>
       <c r="E6" t="n">
-        <v>6892.169921875</v>
+        <v>6840.22998046875</v>
       </c>
       <c r="F6" t="n">
-        <v>-7.0400390625</v>
+        <v>10.52978515625</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Profit</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>6781.4599609375</v>
+        <v>6781.39990234375</v>
       </c>
       <c r="D7" t="n">
         <v>6772.39990234375</v>
@@ -628,7 +628,7 @@
         <v>6772.39990234375</v>
       </c>
       <c r="F7" t="n">
-        <v>-9.06005859375</v>
+        <v>-9</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>6837.10009765625</v>
+        <v>6837.009765625</v>
       </c>
       <c r="D8" t="n">
         <v>6831.81982421875</v>
@@ -655,7 +655,7 @@
         <v>6831.81982421875</v>
       </c>
       <c r="F8" t="n">
-        <v>5.2802734375</v>
+        <v>5.18994140625</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6850.66015625</v>
+        <v>6850.68017578125</v>
       </c>
       <c r="D9" t="n">
         <v>6848.08984375</v>
@@ -682,7 +682,7 @@
         <v>6848.08984375</v>
       </c>
       <c r="F9" t="n">
-        <v>2.5703125</v>
+        <v>2.59033203125</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>6736.3798828125</v>
+        <v>6736.18994140625</v>
       </c>
       <c r="D10" t="n">
         <v>6738.52001953125</v>
@@ -709,7 +709,7 @@
         <v>6738.52001953125</v>
       </c>
       <c r="F10" t="n">
-        <v>2.14013671875</v>
+        <v>2.330078125</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -727,7 +727,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>6656.58984375</v>
+        <v>6656.6201171875</v>
       </c>
       <c r="D11" t="n">
         <v>6672.91015625</v>
@@ -736,7 +736,7 @@
         <v>6672.91015625</v>
       </c>
       <c r="F11" t="n">
-        <v>16.3203125</v>
+        <v>16.2900390625</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>6655.43017578125</v>
+        <v>6655.43994140625</v>
       </c>
       <c r="D12" t="n">
         <v>6616.93994140625</v>
@@ -763,7 +763,7 @@
         <v>6616.93994140625</v>
       </c>
       <c r="F12" t="n">
-        <v>38.490234375</v>
+        <v>38.5</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -773,24 +773,24 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45982</v>
+        <v>45980</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SHORT</t>
+          <t>LONG</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6632.18017578125</v>
+        <v>6638.8701171875</v>
       </c>
       <c r="D13" t="n">
-        <v>6603.7998046875</v>
+        <v>6642.93017578125</v>
       </c>
       <c r="E13" t="n">
-        <v>6603.7998046875</v>
+        <v>6642.93017578125</v>
       </c>
       <c r="F13" t="n">
-        <v>28.38037109375</v>
+        <v>4.06005859375</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -800,7 +800,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45994</v>
+        <v>45982</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -808,16 +808,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6858.240234375</v>
+        <v>6632.2001953125</v>
       </c>
       <c r="D14" t="n">
-        <v>6850.509765625</v>
+        <v>6603.7998046875</v>
       </c>
       <c r="E14" t="n">
-        <v>6850.509765625</v>
+        <v>6603.7998046875</v>
       </c>
       <c r="F14" t="n">
-        <v>7.73046875</v>
+        <v>28.400390625</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -827,34 +827,34 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45999</v>
+        <v>45985</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LONG</t>
+          <t>SHORT</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6837.490234375</v>
+        <v>6700.14013671875</v>
       </c>
       <c r="D15" t="n">
-        <v>6847.83984375</v>
+        <v>6704.669921875</v>
       </c>
       <c r="E15" t="n">
-        <v>6847.83984375</v>
+        <v>6704.669921875</v>
       </c>
       <c r="F15" t="n">
-        <v>10.349609375</v>
+        <v>-4.52978515625</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>Loss</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>46002</v>
+        <v>45986</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -862,16 +862,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>6894.919921875</v>
+        <v>6747.3798828125</v>
       </c>
       <c r="D16" t="n">
-        <v>6902.10009765625</v>
+        <v>6766.10009765625</v>
       </c>
       <c r="E16" t="n">
-        <v>6902.10009765625</v>
+        <v>6766.10009765625</v>
       </c>
       <c r="F16" t="n">
-        <v>-7.18017578125</v>
+        <v>-18.72021484375</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -881,24 +881,24 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>46007</v>
+        <v>45992</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LONG</t>
+          <t>SHORT</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>6787.419921875</v>
+        <v>6819.5498046875</v>
       </c>
       <c r="D17" t="n">
-        <v>6798.509765625</v>
+        <v>6814.64990234375</v>
       </c>
       <c r="E17" t="n">
-        <v>6798.509765625</v>
+        <v>6814.64990234375</v>
       </c>
       <c r="F17" t="n">
-        <v>11.08984375</v>
+        <v>4.89990234375</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -908,34 +908,34 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>46008</v>
+        <v>45994</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LONG</t>
+          <t>SHORT</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>6736.669921875</v>
+        <v>6858.22998046875</v>
       </c>
       <c r="D18" t="n">
-        <v>6722.22021484375</v>
+        <v>6850.509765625</v>
       </c>
       <c r="E18" t="n">
-        <v>6722.22021484375</v>
+        <v>6850.509765625</v>
       </c>
       <c r="F18" t="n">
-        <v>-14.44970703125</v>
+        <v>7.72021484375</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Profit</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>46009</v>
+        <v>45999</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -943,26 +943,26 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>6782.68017578125</v>
+        <v>6837.509765625</v>
       </c>
       <c r="D19" t="n">
-        <v>6774.35009765625</v>
+        <v>6847.83984375</v>
       </c>
       <c r="E19" t="n">
-        <v>6774.35009765625</v>
+        <v>6847.83984375</v>
       </c>
       <c r="F19" t="n">
-        <v>-8.330078125</v>
+        <v>10.330078125</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>Profit</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>46014</v>
+        <v>46001</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -970,16 +970,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6905.83984375</v>
+        <v>6838.14990234375</v>
       </c>
       <c r="D20" t="n">
-        <v>6909.02001953125</v>
+        <v>6886.9501953125</v>
       </c>
       <c r="E20" t="n">
-        <v>6909.02001953125</v>
+        <v>6886.9501953125</v>
       </c>
       <c r="F20" t="n">
-        <v>-3.18017578125</v>
+        <v>-48.80029296875</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -989,51 +989,51 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>46024</v>
+        <v>46002</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LONG</t>
+          <t>SHORT</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>6850.1201171875</v>
+        <v>6895.1298828125</v>
       </c>
       <c r="D21" t="n">
-        <v>6858.5400390625</v>
+        <v>6902.10009765625</v>
       </c>
       <c r="E21" t="n">
-        <v>6858.5400390625</v>
+        <v>6902.10009765625</v>
       </c>
       <c r="F21" t="n">
-        <v>8.419921875</v>
+        <v>-6.97021484375</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>Loss</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>46028</v>
+        <v>46006</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SHORT</t>
+          <t>LONG</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>6944.43994140625</v>
+        <v>6817.14990234375</v>
       </c>
       <c r="D22" t="n">
-        <v>6946.330078125</v>
+        <v>6816.33984375</v>
       </c>
       <c r="E22" t="n">
-        <v>6946.330078125</v>
+        <v>6816.33984375</v>
       </c>
       <c r="F22" t="n">
-        <v>-1.89013671875</v>
+        <v>-0.81005859375</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1043,24 +1043,24 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>46031</v>
+        <v>46007</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SHORT</t>
+          <t>LONG</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6973.7099609375</v>
+        <v>6787.52978515625</v>
       </c>
       <c r="D23" t="n">
-        <v>6965.990234375</v>
+        <v>6798.509765625</v>
       </c>
       <c r="E23" t="n">
-        <v>6965.990234375</v>
+        <v>6798.509765625</v>
       </c>
       <c r="F23" t="n">
-        <v>7.7197265625</v>
+        <v>10.97998046875</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1070,34 +1070,34 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>46034</v>
+        <v>46008</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SHORT</t>
+          <t>LONG</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>6978.89990234375</v>
+        <v>6736.6201171875</v>
       </c>
       <c r="D24" t="n">
-        <v>6976.72021484375</v>
+        <v>6722.22021484375</v>
       </c>
       <c r="E24" t="n">
-        <v>6976.72021484375</v>
+        <v>6722.22021484375</v>
       </c>
       <c r="F24" t="n">
-        <v>2.1796875</v>
+        <v>-14.39990234375</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>Loss</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>46035</v>
+        <v>46009</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1105,45 +1105,288 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>6953.3701171875</v>
+        <v>6784.990234375</v>
       </c>
       <c r="D25" t="n">
-        <v>6962.97998046875</v>
+        <v>6774.35009765625</v>
       </c>
       <c r="E25" t="n">
-        <v>6962.97998046875</v>
+        <v>6774.35009765625</v>
       </c>
       <c r="F25" t="n">
-        <v>9.60986328125</v>
+        <v>-10.64013671875</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>Loss</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
+        <v>46010</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>6831.52978515625</v>
+      </c>
+      <c r="D26" t="n">
+        <v>6834.7001953125</v>
+      </c>
+      <c r="E26" t="n">
+        <v>6834.7001953125</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-3.17041015625</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>46014</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>6905.7900390625</v>
+      </c>
+      <c r="D27" t="n">
+        <v>6909.02001953125</v>
+      </c>
+      <c r="E27" t="n">
+        <v>6909.02001953125</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-3.22998046875</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>46017</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>6930.919921875</v>
+      </c>
+      <c r="D28" t="n">
+        <v>6930.52001953125</v>
+      </c>
+      <c r="E28" t="n">
+        <v>6930.52001953125</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-0.39990234375</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>6850.08984375</v>
+      </c>
+      <c r="D29" t="n">
+        <v>6858.5400390625</v>
+      </c>
+      <c r="E29" t="n">
+        <v>6858.5400390625</v>
+      </c>
+      <c r="F29" t="n">
+        <v>8.4501953125</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>6944.740234375</v>
+      </c>
+      <c r="D30" t="n">
+        <v>6946.330078125</v>
+      </c>
+      <c r="E30" t="n">
+        <v>6946.330078125</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-1.58984375</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>46031</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>6973.68017578125</v>
+      </c>
+      <c r="D31" t="n">
+        <v>6965.990234375</v>
+      </c>
+      <c r="E31" t="n">
+        <v>6965.990234375</v>
+      </c>
+      <c r="F31" t="n">
+        <v>7.68994140625</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>46034</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>6978.7998046875</v>
+      </c>
+      <c r="D32" t="n">
+        <v>6976.72021484375</v>
+      </c>
+      <c r="E32" t="n">
+        <v>6976.72021484375</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2.07958984375</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>46035</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>6955.830078125</v>
+      </c>
+      <c r="D33" t="n">
+        <v>6962.97998046875</v>
+      </c>
+      <c r="E33" t="n">
+        <v>6962.97998046875</v>
+      </c>
+      <c r="F33" t="n">
+        <v>7.14990234375</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
         <v>46036</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>6893.0498046875</v>
-      </c>
-      <c r="D26" t="n">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>6893.08984375</v>
+      </c>
+      <c r="D34" t="n">
         <v>6928.41015625</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E34" t="n">
         <v>6928.41015625</v>
       </c>
-      <c r="F26" t="n">
-        <v>35.3603515625</v>
-      </c>
-      <c r="G26" t="inlineStr">
+      <c r="F34" t="n">
+        <v>35.3203125</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>46037</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SHORT</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>6967.9599609375</v>
+      </c>
+      <c r="D35" t="n">
+        <v>6944.97021484375</v>
+      </c>
+      <c r="E35" t="n">
+        <v>6944.97021484375</v>
+      </c>
+      <c r="F35" t="n">
+        <v>22.98974609375</v>
+      </c>
+      <c r="G35" t="inlineStr">
         <is>
           <t>Profit</t>
         </is>

</xml_diff>

<commit_message>
Update README and strategy settings
</commit_message>
<xml_diff>
--- a/trade_log.xlsx
+++ b/trade_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,22 +445,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>Entry</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Entry</t>
+          <t>Exit</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Exit</t>
+          <t>Close</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Close</t>
+          <t>Exit Reason</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -470,925 +470,682 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Result</t>
+          <t>Win Rate</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45952</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>45954</v>
+      </c>
+      <c r="B2" t="n">
+        <v>6804.35986328125</v>
       </c>
       <c r="C2" t="n">
-        <v>6678.3701171875</v>
+        <v>6791.14013671875</v>
       </c>
       <c r="D2" t="n">
-        <v>6699.77978515625</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6699.77978515625</v>
+        <v>6791.14013671875</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F2" t="n">
-        <v>21.40966796875</v>
+        <v>13.2197265625</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45953</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>45968</v>
+      </c>
+      <c r="B3" t="n">
+        <v>6665.3798828125</v>
       </c>
       <c r="C3" t="n">
-        <v>6747.14990234375</v>
+        <v>6729.02001953125</v>
       </c>
       <c r="D3" t="n">
-        <v>6738.169921875</v>
-      </c>
-      <c r="E3" t="n">
-        <v>6738.169921875</v>
+        <v>6729.02001953125</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F3" t="n">
-        <v>8.97998046875</v>
+        <v>63.64013671875</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45954</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>45971</v>
+      </c>
+      <c r="B4" t="n">
+        <v>6786.83984375</v>
       </c>
       <c r="C4" t="n">
-        <v>6804.06005859375</v>
+        <v>6831.81982421875</v>
       </c>
       <c r="D4" t="n">
-        <v>6791.14013671875</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6791.14013671875</v>
+        <v>6831.81982421875</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F4" t="n">
-        <v>12.919921875</v>
+        <v>44.97998046875</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45959</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>45972</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6817.06982421875</v>
       </c>
       <c r="C5" t="n">
-        <v>6899.18017578125</v>
+        <v>6848.08984375</v>
       </c>
       <c r="D5" t="n">
-        <v>6892.169921875</v>
-      </c>
-      <c r="E5" t="n">
-        <v>6892.169921875</v>
+        <v>6848.08984375</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F5" t="n">
-        <v>-7.01025390625</v>
+        <v>31.02001953125</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45961</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>45973</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6843.58984375</v>
       </c>
       <c r="C6" t="n">
-        <v>6829.7001953125</v>
+        <v>6852</v>
       </c>
       <c r="D6" t="n">
-        <v>6840.22998046875</v>
-      </c>
-      <c r="E6" t="n">
-        <v>6840.22998046875</v>
+        <v>6852</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F6" t="n">
-        <v>10.52978515625</v>
+        <v>8.41015625</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45965</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>45974</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6765.02001953125</v>
       </c>
       <c r="C7" t="n">
-        <v>6781.39990234375</v>
+        <v>6738.52001953125</v>
       </c>
       <c r="D7" t="n">
-        <v>6772.39990234375</v>
-      </c>
-      <c r="E7" t="n">
-        <v>6772.39990234375</v>
+        <v>6738.52001953125</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F7" t="n">
-        <v>-9</v>
+        <v>-26.5</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45971</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>45978</v>
+      </c>
+      <c r="B8" t="n">
+        <v>6682.5400390625</v>
       </c>
       <c r="C8" t="n">
-        <v>6837.009765625</v>
+        <v>6672.91015625</v>
       </c>
       <c r="D8" t="n">
-        <v>6831.81982421875</v>
-      </c>
-      <c r="E8" t="n">
-        <v>6831.81982421875</v>
+        <v>6672.91015625</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F8" t="n">
-        <v>5.18994140625</v>
+        <v>-9.6298828125</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45972</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>45980</v>
+      </c>
+      <c r="B9" t="n">
+        <v>6640.68994140625</v>
       </c>
       <c r="C9" t="n">
-        <v>6850.68017578125</v>
+        <v>6642.93017578125</v>
       </c>
       <c r="D9" t="n">
-        <v>6848.08984375</v>
-      </c>
-      <c r="E9" t="n">
-        <v>6848.08984375</v>
+        <v>6642.93017578125</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F9" t="n">
-        <v>2.59033203125</v>
+        <v>2.240234375</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45974</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>45985</v>
+      </c>
+      <c r="B10" t="n">
+        <v>6687.2001953125</v>
       </c>
       <c r="C10" t="n">
-        <v>6736.18994140625</v>
+        <v>6704.669921875</v>
       </c>
       <c r="D10" t="n">
-        <v>6738.52001953125</v>
-      </c>
-      <c r="E10" t="n">
-        <v>6738.52001953125</v>
+        <v>6704.669921875</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F10" t="n">
-        <v>2.330078125</v>
+        <v>-17.4697265625</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45978</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>45987</v>
+      </c>
+      <c r="B11" t="n">
+        <v>6822.22021484375</v>
       </c>
       <c r="C11" t="n">
-        <v>6656.6201171875</v>
+        <v>6811.759765625</v>
       </c>
       <c r="D11" t="n">
-        <v>6672.91015625</v>
-      </c>
-      <c r="E11" t="n">
-        <v>6672.91015625</v>
+        <v>6811.759765625</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F11" t="n">
-        <v>16.2900390625</v>
+        <v>10.46044921875</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45979</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>45989</v>
+      </c>
+      <c r="B12" t="n">
+        <v>6842.08984375</v>
       </c>
       <c r="C12" t="n">
-        <v>6655.43994140625</v>
+        <v>6848.47998046875</v>
       </c>
       <c r="D12" t="n">
-        <v>6616.93994140625</v>
-      </c>
-      <c r="E12" t="n">
-        <v>6616.93994140625</v>
+        <v>6848.47998046875</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F12" t="n">
-        <v>38.5</v>
+        <v>-6.39013671875</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45980</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>45992</v>
+      </c>
+      <c r="B13" t="n">
+        <v>6833.89013671875</v>
       </c>
       <c r="C13" t="n">
-        <v>6638.8701171875</v>
+        <v>6814.64990234375</v>
       </c>
       <c r="D13" t="n">
-        <v>6642.93017578125</v>
-      </c>
-      <c r="E13" t="n">
-        <v>6642.93017578125</v>
+        <v>6814.64990234375</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F13" t="n">
-        <v>4.06005859375</v>
+        <v>19.240234375</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45982</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>45993</v>
+      </c>
+      <c r="B14" t="n">
+        <v>6824.22021484375</v>
       </c>
       <c r="C14" t="n">
-        <v>6632.2001953125</v>
+        <v>6827.830078125</v>
       </c>
       <c r="D14" t="n">
-        <v>6603.7998046875</v>
-      </c>
-      <c r="E14" t="n">
-        <v>6603.7998046875</v>
+        <v>6827.830078125</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F14" t="n">
-        <v>28.400390625</v>
+        <v>3.60986328125</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45985</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>45995</v>
+      </c>
+      <c r="B15" t="n">
+        <v>6856.81982421875</v>
       </c>
       <c r="C15" t="n">
-        <v>6700.14013671875</v>
+        <v>6857.9599609375</v>
       </c>
       <c r="D15" t="n">
-        <v>6704.669921875</v>
-      </c>
-      <c r="E15" t="n">
-        <v>6704.669921875</v>
+        <v>6857.9599609375</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F15" t="n">
-        <v>-4.52978515625</v>
+        <v>1.14013671875</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45986</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>46000</v>
+      </c>
+      <c r="B16" t="n">
+        <v>6854.14013671875</v>
       </c>
       <c r="C16" t="n">
-        <v>6747.3798828125</v>
+        <v>6840.31982421875</v>
       </c>
       <c r="D16" t="n">
-        <v>6766.10009765625</v>
-      </c>
-      <c r="E16" t="n">
-        <v>6766.10009765625</v>
+        <v>6840.31982421875</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F16" t="n">
-        <v>-18.72021484375</v>
+        <v>13.8203125</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45992</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>46001</v>
+      </c>
+      <c r="B17" t="n">
+        <v>6847.16015625</v>
       </c>
       <c r="C17" t="n">
-        <v>6819.5498046875</v>
+        <v>6886.9501953125</v>
       </c>
       <c r="D17" t="n">
-        <v>6814.64990234375</v>
-      </c>
-      <c r="E17" t="n">
-        <v>6814.64990234375</v>
+        <v>6886.9501953125</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F17" t="n">
-        <v>4.89990234375</v>
+        <v>-39.7900390625</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45994</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>46006</v>
+      </c>
+      <c r="B18" t="n">
+        <v>6819.77001953125</v>
       </c>
       <c r="C18" t="n">
-        <v>6858.22998046875</v>
+        <v>6816.33984375</v>
       </c>
       <c r="D18" t="n">
-        <v>6850.509765625</v>
-      </c>
-      <c r="E18" t="n">
-        <v>6850.509765625</v>
+        <v>6816.33984375</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F18" t="n">
-        <v>7.72021484375</v>
+        <v>-3.43017578125</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45999</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>46007</v>
+      </c>
+      <c r="B19" t="n">
+        <v>6792.2001953125</v>
       </c>
       <c r="C19" t="n">
-        <v>6837.509765625</v>
+        <v>6798.509765625</v>
       </c>
       <c r="D19" t="n">
-        <v>6847.83984375</v>
-      </c>
-      <c r="E19" t="n">
-        <v>6847.83984375</v>
+        <v>6798.509765625</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F19" t="n">
-        <v>10.330078125</v>
+        <v>6.3095703125</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>46001</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>46009</v>
+      </c>
+      <c r="B20" t="n">
+        <v>6804.990234375</v>
       </c>
       <c r="C20" t="n">
-        <v>6838.14990234375</v>
+        <v>6774.35009765625</v>
       </c>
       <c r="D20" t="n">
-        <v>6886.9501953125</v>
-      </c>
-      <c r="E20" t="n">
-        <v>6886.9501953125</v>
+        <v>6774.35009765625</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F20" t="n">
-        <v>-48.80029296875</v>
+        <v>30.64013671875</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>46002</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>46017</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6930.72021484375</v>
       </c>
       <c r="C21" t="n">
-        <v>6895.1298828125</v>
+        <v>6930.52001953125</v>
       </c>
       <c r="D21" t="n">
-        <v>6902.10009765625</v>
-      </c>
-      <c r="E21" t="n">
-        <v>6902.10009765625</v>
+        <v>6930.52001953125</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F21" t="n">
-        <v>-6.97021484375</v>
+        <v>-0.2001953125</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>46006</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>46020</v>
+      </c>
+      <c r="B22" t="n">
+        <v>6900.97998046875</v>
       </c>
       <c r="C22" t="n">
-        <v>6817.14990234375</v>
+        <v>6906.9599609375</v>
       </c>
       <c r="D22" t="n">
-        <v>6816.33984375</v>
-      </c>
-      <c r="E22" t="n">
-        <v>6816.33984375</v>
+        <v>6906.9599609375</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F22" t="n">
-        <v>-0.81005859375</v>
+        <v>5.97998046875</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>46007</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>46021</v>
+      </c>
+      <c r="B23" t="n">
+        <v>6900.14990234375</v>
       </c>
       <c r="C23" t="n">
-        <v>6787.52978515625</v>
+        <v>6896.4501953125</v>
       </c>
       <c r="D23" t="n">
-        <v>6798.509765625</v>
-      </c>
-      <c r="E23" t="n">
-        <v>6798.509765625</v>
+        <v>6896.4501953125</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F23" t="n">
-        <v>10.97998046875</v>
+        <v>3.69970703125</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>46008</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>46035</v>
+      </c>
+      <c r="B24" t="n">
+        <v>6954.6201171875</v>
       </c>
       <c r="C24" t="n">
-        <v>6736.6201171875</v>
+        <v>6962.97998046875</v>
       </c>
       <c r="D24" t="n">
-        <v>6722.22021484375</v>
-      </c>
-      <c r="E24" t="n">
-        <v>6722.22021484375</v>
+        <v>6962.97998046875</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F24" t="n">
-        <v>-14.39990234375</v>
+        <v>8.35986328125</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>46009</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
+        <v>46036</v>
+      </c>
+      <c r="B25" t="n">
+        <v>6893.08984375</v>
       </c>
       <c r="C25" t="n">
-        <v>6784.990234375</v>
+        <v>6928.41015625</v>
       </c>
       <c r="D25" t="n">
-        <v>6774.35009765625</v>
-      </c>
-      <c r="E25" t="n">
-        <v>6774.35009765625</v>
+        <v>6928.41015625</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F25" t="n">
-        <v>-10.64013671875</v>
+        <v>35.3203125</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Loss</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>46010</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
+        <v>46037</v>
+      </c>
+      <c r="B26" t="n">
+        <v>6972.10009765625</v>
       </c>
       <c r="C26" t="n">
-        <v>6831.52978515625</v>
+        <v>6944.97021484375</v>
       </c>
       <c r="D26" t="n">
-        <v>6834.7001953125</v>
-      </c>
-      <c r="E26" t="n">
-        <v>6834.7001953125</v>
+        <v>6944.97021484375</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Closing Price</t>
+        </is>
       </c>
       <c r="F26" t="n">
-        <v>-3.17041015625</v>
+        <v>27.1298828125</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Loss</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
-        <v>46014</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>6905.7900390625</v>
-      </c>
-      <c r="D27" t="n">
-        <v>6909.02001953125</v>
-      </c>
-      <c r="E27" t="n">
-        <v>6909.02001953125</v>
-      </c>
-      <c r="F27" t="n">
-        <v>-3.22998046875</v>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Loss</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
-        <v>46017</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>6930.919921875</v>
-      </c>
-      <c r="D28" t="n">
-        <v>6930.52001953125</v>
-      </c>
-      <c r="E28" t="n">
-        <v>6930.52001953125</v>
-      </c>
-      <c r="F28" t="n">
-        <v>-0.39990234375</v>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Loss</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="n">
-        <v>46024</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>6850.08984375</v>
-      </c>
-      <c r="D29" t="n">
-        <v>6858.5400390625</v>
-      </c>
-      <c r="E29" t="n">
-        <v>6858.5400390625</v>
-      </c>
-      <c r="F29" t="n">
-        <v>8.4501953125</v>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="n">
-        <v>46028</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>6944.740234375</v>
-      </c>
-      <c r="D30" t="n">
-        <v>6946.330078125</v>
-      </c>
-      <c r="E30" t="n">
-        <v>6946.330078125</v>
-      </c>
-      <c r="F30" t="n">
-        <v>-1.58984375</v>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Loss</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="n">
-        <v>46031</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>6973.68017578125</v>
-      </c>
-      <c r="D31" t="n">
-        <v>6965.990234375</v>
-      </c>
-      <c r="E31" t="n">
-        <v>6965.990234375</v>
-      </c>
-      <c r="F31" t="n">
-        <v>7.68994140625</v>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="n">
-        <v>46034</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>6978.7998046875</v>
-      </c>
-      <c r="D32" t="n">
-        <v>6976.72021484375</v>
-      </c>
-      <c r="E32" t="n">
-        <v>6976.72021484375</v>
-      </c>
-      <c r="F32" t="n">
-        <v>2.07958984375</v>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="n">
-        <v>46035</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>6955.830078125</v>
-      </c>
-      <c r="D33" t="n">
-        <v>6962.97998046875</v>
-      </c>
-      <c r="E33" t="n">
-        <v>6962.97998046875</v>
-      </c>
-      <c r="F33" t="n">
-        <v>7.14990234375</v>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="n">
-        <v>46036</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>LONG</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>6893.08984375</v>
-      </c>
-      <c r="D34" t="n">
-        <v>6928.41015625</v>
-      </c>
-      <c r="E34" t="n">
-        <v>6928.41015625</v>
-      </c>
-      <c r="F34" t="n">
-        <v>35.3203125</v>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="n">
-        <v>46037</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>SHORT</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>6967.9599609375</v>
-      </c>
-      <c r="D35" t="n">
-        <v>6944.97021484375</v>
-      </c>
-      <c r="E35" t="n">
-        <v>6944.97021484375</v>
-      </c>
-      <c r="F35" t="n">
-        <v>22.98974609375</v>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Profit</t>
+          <t>72.00%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update strategy to exit at support/resistance levels
</commit_message>
<xml_diff>
--- a/trade_log.xlsx
+++ b/trade_log.xlsx
@@ -509,18 +509,18 @@
         <v>6665.3798828125</v>
       </c>
       <c r="C3" t="n">
-        <v>6729.02001953125</v>
+        <v>6696.18017578125</v>
       </c>
       <c r="D3" t="n">
         <v>6729.02001953125</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Closing Price</t>
+          <t>Resistance Level</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>63.64013671875</v>
+        <v>30.80029296875</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -536,18 +536,18 @@
         <v>6786.83984375</v>
       </c>
       <c r="C4" t="n">
-        <v>6831.81982421875</v>
+        <v>6808.9501953125</v>
       </c>
       <c r="D4" t="n">
         <v>6831.81982421875</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Closing Price</t>
+          <t>Resistance Level</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>44.97998046875</v>
+        <v>22.1103515625</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -563,18 +563,18 @@
         <v>6817.06982421875</v>
       </c>
       <c r="C5" t="n">
-        <v>6848.08984375</v>
+        <v>6827.31005859375</v>
       </c>
       <c r="D5" t="n">
         <v>6848.08984375</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Closing Price</t>
+          <t>Resistance Level</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>31.02001953125</v>
+        <v>10.240234375</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -860,18 +860,18 @@
         <v>6854.14013671875</v>
       </c>
       <c r="C16" t="n">
-        <v>6840.31982421875</v>
+        <v>6840.60986328125</v>
       </c>
       <c r="D16" t="n">
         <v>6840.31982421875</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Closing Price</t>
+          <t>Support Level</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>13.8203125</v>
+        <v>13.5302734375</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -968,18 +968,18 @@
         <v>6804.990234375</v>
       </c>
       <c r="C20" t="n">
-        <v>6774.35009765625</v>
+        <v>6771.72021484375</v>
       </c>
       <c r="D20" t="n">
         <v>6774.35009765625</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Closing Price</t>
+          <t>Support Level</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>30.64013671875</v>
+        <v>33.27001953125</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1022,18 +1022,18 @@
         <v>6900.97998046875</v>
       </c>
       <c r="C22" t="n">
-        <v>6906.9599609375</v>
+        <v>6912.6201171875</v>
       </c>
       <c r="D22" t="n">
         <v>6906.9599609375</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Closing Price</t>
+          <t>Resistance Level</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>5.97998046875</v>
+        <v>11.64013671875</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1049,18 +1049,18 @@
         <v>6900.14990234375</v>
       </c>
       <c r="C23" t="n">
-        <v>6896.4501953125</v>
+        <v>6895.2998046875</v>
       </c>
       <c r="D23" t="n">
         <v>6896.4501953125</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Closing Price</t>
+          <t>Support Level</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>3.69970703125</v>
+        <v>4.85009765625</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1130,18 +1130,18 @@
         <v>6972.10009765625</v>
       </c>
       <c r="C26" t="n">
-        <v>6944.97021484375</v>
+        <v>6960.81005859375</v>
       </c>
       <c r="D26" t="n">
         <v>6944.97021484375</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Closing Price</t>
+          <t>Support Level</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>27.1298828125</v>
+        <v>11.2900390625</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update exit logic to confirmed exit at support/resistance levels
</commit_message>
<xml_diff>
--- a/trade_log.xlsx
+++ b/trade_log.xlsx
@@ -509,18 +509,18 @@
         <v>6665.3798828125</v>
       </c>
       <c r="C3" t="n">
-        <v>6696.18017578125</v>
+        <v>6714.7900390625</v>
       </c>
       <c r="D3" t="n">
         <v>6729.02001953125</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Resistance Level</t>
+          <t>Resistance Confirmed</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>30.80029296875</v>
+        <v>49.41015625</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -536,18 +536,18 @@
         <v>6786.83984375</v>
       </c>
       <c r="C4" t="n">
-        <v>6808.9501953125</v>
+        <v>6839.72998046875</v>
       </c>
       <c r="D4" t="n">
         <v>6831.81982421875</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Resistance Level</t>
+          <t>Resistance Confirmed</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>22.1103515625</v>
+        <v>52.89013671875</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -563,18 +563,18 @@
         <v>6817.06982421875</v>
       </c>
       <c r="C5" t="n">
-        <v>6827.31005859375</v>
+        <v>6848.33984375</v>
       </c>
       <c r="D5" t="n">
         <v>6848.08984375</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Resistance Level</t>
+          <t>Resistance Confirmed</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>10.240234375</v>
+        <v>31.27001953125</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -860,18 +860,18 @@
         <v>6854.14013671875</v>
       </c>
       <c r="C16" t="n">
-        <v>6840.60986328125</v>
+        <v>6840.31982421875</v>
       </c>
       <c r="D16" t="n">
         <v>6840.31982421875</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Support Level</t>
+          <t>Closing Price</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>13.5302734375</v>
+        <v>13.8203125</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -968,18 +968,18 @@
         <v>6804.990234375</v>
       </c>
       <c r="C20" t="n">
-        <v>6771.72021484375</v>
+        <v>6767.27001953125</v>
       </c>
       <c r="D20" t="n">
         <v>6774.35009765625</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Support Level</t>
+          <t>Support Confirmed</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>33.27001953125</v>
+        <v>37.72021484375</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1022,18 +1022,18 @@
         <v>6900.97998046875</v>
       </c>
       <c r="C22" t="n">
-        <v>6912.6201171875</v>
+        <v>6909.740234375</v>
       </c>
       <c r="D22" t="n">
         <v>6906.9599609375</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Resistance Level</t>
+          <t>Resistance Confirmed</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>11.64013671875</v>
+        <v>8.76025390625</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1049,18 +1049,18 @@
         <v>6900.14990234375</v>
       </c>
       <c r="C23" t="n">
-        <v>6895.2998046875</v>
+        <v>6896.4501953125</v>
       </c>
       <c r="D23" t="n">
         <v>6896.4501953125</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Support Level</t>
+          <t>Closing Price</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>4.85009765625</v>
+        <v>3.69970703125</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1130,18 +1130,18 @@
         <v>6972.10009765625</v>
       </c>
       <c r="C26" t="n">
-        <v>6960.81005859375</v>
+        <v>6944.97021484375</v>
       </c>
       <c r="D26" t="n">
         <v>6944.97021484375</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Support Level</t>
+          <t>Closing Price</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>11.2900390625</v>
+        <v>27.1298828125</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>

</xml_diff>